<commit_message>
Documentação e comentarios no codigo
Processo de implementação de macro no resultado da aplicação ainda em andamento
</commit_message>
<xml_diff>
--- a/uploads/Fechamento_preenchido.xlsx
+++ b/uploads/Fechamento_preenchido.xlsx
@@ -58721,7 +58721,7 @@
         </is>
       </c>
       <c r="D869" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E869" t="inlineStr"/>
       <c r="F869" t="inlineStr"/>
@@ -58757,7 +58757,7 @@
         </is>
       </c>
       <c r="D870" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E870" t="inlineStr"/>
       <c r="F870" t="inlineStr"/>
@@ -58793,7 +58793,7 @@
         </is>
       </c>
       <c r="D871" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E871" t="inlineStr"/>
       <c r="F871" t="inlineStr"/>
@@ -58829,7 +58829,7 @@
         </is>
       </c>
       <c r="D872" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E872" t="inlineStr"/>
       <c r="F872" t="inlineStr"/>
@@ -58865,7 +58865,7 @@
         </is>
       </c>
       <c r="D873" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E873" t="inlineStr"/>
       <c r="F873" t="inlineStr"/>
@@ -58901,7 +58901,7 @@
         </is>
       </c>
       <c r="D874" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E874" t="inlineStr"/>
       <c r="F874" t="inlineStr"/>
@@ -58937,7 +58937,7 @@
         </is>
       </c>
       <c r="D875" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E875" t="inlineStr"/>
       <c r="F875" t="inlineStr"/>
@@ -58973,7 +58973,7 @@
         </is>
       </c>
       <c r="D876" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E876" t="inlineStr"/>
       <c r="F876" t="inlineStr"/>
@@ -59009,7 +59009,7 @@
         </is>
       </c>
       <c r="D877" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E877" t="inlineStr"/>
       <c r="F877" t="inlineStr"/>
@@ -59045,7 +59045,7 @@
         </is>
       </c>
       <c r="D878" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E878" t="inlineStr"/>
       <c r="F878" t="inlineStr"/>
@@ -59081,7 +59081,7 @@
         </is>
       </c>
       <c r="D879" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E879" t="inlineStr"/>
       <c r="F879" t="inlineStr"/>
@@ -59117,7 +59117,7 @@
         </is>
       </c>
       <c r="D880" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E880" t="inlineStr"/>
       <c r="F880" t="inlineStr"/>
@@ -59153,7 +59153,7 @@
         </is>
       </c>
       <c r="D881" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E881" t="inlineStr"/>
       <c r="F881" t="inlineStr"/>
@@ -59189,7 +59189,7 @@
         </is>
       </c>
       <c r="D882" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E882" t="inlineStr"/>
       <c r="F882" t="inlineStr"/>
@@ -59225,7 +59225,7 @@
         </is>
       </c>
       <c r="D883" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E883" t="inlineStr"/>
       <c r="F883" t="inlineStr"/>
@@ -59261,7 +59261,7 @@
         </is>
       </c>
       <c r="D884" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E884" t="inlineStr"/>
       <c r="F884" t="inlineStr"/>
@@ -59297,7 +59297,7 @@
         </is>
       </c>
       <c r="D885" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E885" t="inlineStr"/>
       <c r="F885" t="inlineStr"/>
@@ -59333,7 +59333,7 @@
         </is>
       </c>
       <c r="D886" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E886" t="inlineStr"/>
       <c r="F886" t="inlineStr"/>
@@ -59369,7 +59369,7 @@
         </is>
       </c>
       <c r="D887" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E887" t="inlineStr"/>
       <c r="F887" t="inlineStr"/>
@@ -59405,7 +59405,7 @@
         </is>
       </c>
       <c r="D888" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E888" t="inlineStr"/>
       <c r="F888" t="inlineStr"/>
@@ -59441,7 +59441,7 @@
         </is>
       </c>
       <c r="D889" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E889" t="inlineStr"/>
       <c r="F889" t="inlineStr"/>
@@ -59477,7 +59477,7 @@
         </is>
       </c>
       <c r="D890" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E890" t="inlineStr"/>
       <c r="F890" t="inlineStr"/>
@@ -59513,7 +59513,7 @@
         </is>
       </c>
       <c r="D891" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E891" t="inlineStr"/>
       <c r="F891" t="inlineStr"/>
@@ -59549,7 +59549,7 @@
         </is>
       </c>
       <c r="D892" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E892" t="inlineStr"/>
       <c r="F892" t="inlineStr"/>
@@ -59585,7 +59585,7 @@
         </is>
       </c>
       <c r="D893" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E893" t="inlineStr"/>
       <c r="F893" t="inlineStr"/>
@@ -59621,7 +59621,7 @@
         </is>
       </c>
       <c r="D894" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E894" t="inlineStr"/>
       <c r="F894" t="inlineStr"/>
@@ -59657,7 +59657,7 @@
         </is>
       </c>
       <c r="D895" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E895" t="inlineStr"/>
       <c r="F895" t="inlineStr"/>
@@ -59693,7 +59693,7 @@
         </is>
       </c>
       <c r="D896" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E896" t="inlineStr"/>
       <c r="F896" t="inlineStr"/>
@@ -59729,7 +59729,7 @@
         </is>
       </c>
       <c r="D897" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E897" t="inlineStr"/>
       <c r="F897" t="inlineStr"/>
@@ -59765,7 +59765,7 @@
         </is>
       </c>
       <c r="D898" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E898" t="inlineStr"/>
       <c r="F898" t="inlineStr"/>
@@ -59801,7 +59801,7 @@
         </is>
       </c>
       <c r="D899" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E899" t="inlineStr"/>
       <c r="F899" t="inlineStr"/>
@@ -59837,7 +59837,7 @@
         </is>
       </c>
       <c r="D900" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E900" t="inlineStr"/>
       <c r="F900" t="inlineStr"/>
@@ -59873,7 +59873,7 @@
         </is>
       </c>
       <c r="D901" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E901" t="inlineStr"/>
       <c r="F901" t="inlineStr"/>
@@ -59909,7 +59909,7 @@
         </is>
       </c>
       <c r="D902" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E902" t="inlineStr"/>
       <c r="F902" t="inlineStr"/>
@@ -59945,7 +59945,7 @@
         </is>
       </c>
       <c r="D903" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E903" t="inlineStr"/>
       <c r="F903" t="inlineStr"/>
@@ -59981,7 +59981,7 @@
         </is>
       </c>
       <c r="D904" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E904" t="inlineStr"/>
       <c r="F904" t="inlineStr"/>
@@ -60017,7 +60017,7 @@
         </is>
       </c>
       <c r="D905" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E905" t="inlineStr"/>
       <c r="F905" t="inlineStr"/>
@@ -60053,7 +60053,7 @@
         </is>
       </c>
       <c r="D906" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E906" t="inlineStr"/>
       <c r="F906" t="inlineStr"/>
@@ -60089,7 +60089,7 @@
         </is>
       </c>
       <c r="D907" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E907" t="inlineStr"/>
       <c r="F907" t="inlineStr"/>
@@ -60125,7 +60125,7 @@
         </is>
       </c>
       <c r="D908" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E908" t="inlineStr"/>
       <c r="F908" t="inlineStr"/>
@@ -60161,7 +60161,7 @@
         </is>
       </c>
       <c r="D909" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E909" t="inlineStr"/>
       <c r="F909" t="inlineStr"/>
@@ -60197,7 +60197,7 @@
         </is>
       </c>
       <c r="D910" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E910" t="inlineStr"/>
       <c r="F910" t="inlineStr"/>
@@ -60233,7 +60233,7 @@
         </is>
       </c>
       <c r="D911" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E911" t="inlineStr"/>
       <c r="F911" t="inlineStr"/>
@@ -60269,7 +60269,7 @@
         </is>
       </c>
       <c r="D912" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E912" t="inlineStr"/>
       <c r="F912" t="inlineStr"/>
@@ -60305,7 +60305,7 @@
         </is>
       </c>
       <c r="D913" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E913" t="inlineStr"/>
       <c r="F913" t="inlineStr"/>
@@ -60341,7 +60341,7 @@
         </is>
       </c>
       <c r="D914" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E914" t="inlineStr"/>
       <c r="F914" t="inlineStr"/>
@@ -60377,7 +60377,7 @@
         </is>
       </c>
       <c r="D915" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E915" t="inlineStr"/>
       <c r="F915" t="inlineStr"/>
@@ -60413,7 +60413,7 @@
         </is>
       </c>
       <c r="D916" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E916" t="inlineStr"/>
       <c r="F916" t="inlineStr"/>
@@ -60449,7 +60449,7 @@
         </is>
       </c>
       <c r="D917" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E917" t="inlineStr"/>
       <c r="F917" t="inlineStr"/>
@@ -60485,7 +60485,7 @@
         </is>
       </c>
       <c r="D918" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E918" t="inlineStr"/>
       <c r="F918" t="inlineStr"/>
@@ -60521,7 +60521,7 @@
         </is>
       </c>
       <c r="D919" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E919" t="inlineStr"/>
       <c r="F919" t="inlineStr"/>
@@ -60557,7 +60557,7 @@
         </is>
       </c>
       <c r="D920" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E920" t="inlineStr"/>
       <c r="F920" t="inlineStr"/>
@@ -60593,7 +60593,7 @@
         </is>
       </c>
       <c r="D921" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E921" t="inlineStr"/>
       <c r="F921" t="inlineStr"/>
@@ -60629,7 +60629,7 @@
         </is>
       </c>
       <c r="D922" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E922" t="inlineStr"/>
       <c r="F922" t="inlineStr"/>
@@ -60665,7 +60665,7 @@
         </is>
       </c>
       <c r="D923" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E923" t="inlineStr"/>
       <c r="F923" t="inlineStr"/>
@@ -60701,7 +60701,7 @@
         </is>
       </c>
       <c r="D924" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E924" t="inlineStr"/>
       <c r="F924" t="inlineStr"/>
@@ -60737,7 +60737,7 @@
         </is>
       </c>
       <c r="D925" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E925" t="inlineStr"/>
       <c r="F925" t="inlineStr"/>
@@ -60773,7 +60773,7 @@
         </is>
       </c>
       <c r="D926" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E926" t="inlineStr"/>
       <c r="F926" t="inlineStr"/>
@@ -60809,7 +60809,7 @@
         </is>
       </c>
       <c r="D927" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E927" t="inlineStr"/>
       <c r="F927" t="inlineStr"/>
@@ -60845,7 +60845,7 @@
         </is>
       </c>
       <c r="D928" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E928" t="inlineStr"/>
       <c r="F928" t="inlineStr"/>
@@ -60881,7 +60881,7 @@
         </is>
       </c>
       <c r="D929" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E929" t="inlineStr"/>
       <c r="F929" t="inlineStr"/>
@@ -60917,7 +60917,7 @@
         </is>
       </c>
       <c r="D930" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E930" t="inlineStr"/>
       <c r="F930" t="inlineStr"/>
@@ -60953,7 +60953,7 @@
         </is>
       </c>
       <c r="D931" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E931" t="inlineStr"/>
       <c r="F931" t="inlineStr"/>
@@ -60989,7 +60989,7 @@
         </is>
       </c>
       <c r="D932" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E932" t="inlineStr"/>
       <c r="F932" t="inlineStr"/>
@@ -61025,7 +61025,7 @@
         </is>
       </c>
       <c r="D933" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E933" t="inlineStr"/>
       <c r="F933" t="inlineStr"/>
@@ -61061,7 +61061,7 @@
         </is>
       </c>
       <c r="D934" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E934" t="inlineStr"/>
       <c r="F934" t="inlineStr"/>
@@ -61097,7 +61097,7 @@
         </is>
       </c>
       <c r="D935" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E935" t="inlineStr"/>
       <c r="F935" t="inlineStr"/>
@@ -61133,7 +61133,7 @@
         </is>
       </c>
       <c r="D936" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E936" t="inlineStr"/>
       <c r="F936" t="inlineStr"/>
@@ -61165,7 +61165,7 @@
         </is>
       </c>
       <c r="D937" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E937" t="inlineStr"/>
       <c r="F937" t="inlineStr"/>
@@ -61201,7 +61201,7 @@
         </is>
       </c>
       <c r="D938" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E938" t="inlineStr"/>
       <c r="F938" t="inlineStr"/>
@@ -61237,7 +61237,7 @@
         </is>
       </c>
       <c r="D939" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E939" t="inlineStr"/>
       <c r="F939" t="inlineStr"/>
@@ -61273,7 +61273,7 @@
         </is>
       </c>
       <c r="D940" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E940" t="inlineStr"/>
       <c r="F940" t="inlineStr"/>
@@ -61309,7 +61309,7 @@
         </is>
       </c>
       <c r="D941" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E941" t="inlineStr"/>
       <c r="F941" t="inlineStr"/>
@@ -61345,7 +61345,7 @@
         </is>
       </c>
       <c r="D942" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E942" t="inlineStr"/>
       <c r="F942" t="inlineStr"/>
@@ -61381,7 +61381,7 @@
         </is>
       </c>
       <c r="D943" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E943" t="inlineStr"/>
       <c r="F943" t="inlineStr"/>
@@ -61417,7 +61417,7 @@
         </is>
       </c>
       <c r="D944" s="3" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="E944" t="inlineStr"/>
       <c r="F944" t="inlineStr"/>

</xml_diff>